<commit_message>
Home-Report:ALPHALIST Annual report added.
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_3.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_3.xlsx
@@ -536,7 +536,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +626,7 @@
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
     </row>
-    <row r="8" spans="1:9" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>

</xml_diff>